<commit_message>
Ajouts de fichiers au rapport
</commit_message>
<xml_diff>
--- a/ressources/analyse/Audit-SEO.xlsx
+++ b/ressources/analyse/Audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="82">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">Spécifier la langue du document</t>
   </si>
   <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Attributs_universels/lang</t>
+  </si>
+  <si>
     <t xml:space="preserve">page2.html</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t xml:space="preserve">Supprimer la répétition</t>
   </si>
   <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/meta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Balise keywords vide</t>
   </si>
   <si>
@@ -112,6 +118,9 @@
     <t xml:space="preserve">Donner un titre descriptif de la page</t>
   </si>
   <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/title</t>
+  </si>
+  <si>
     <t xml:space="preserve">/</t>
   </si>
   <si>
@@ -133,6 +142,9 @@
     <t xml:space="preserve">Utiliser un nom significatif</t>
   </si>
   <si>
+    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Web/HTML/Global_attributes/id</t>
+  </si>
+  <si>
     <t xml:space="preserve">Texte superflu pour augmenter le référencement</t>
   </si>
   <si>
@@ -184,9 +196,6 @@
     <t xml:space="preserve">Traduire le texte en français</t>
   </si>
   <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
     <t xml:space="preserve">« http://www. » est manquant</t>
   </si>
   <si>
@@ -245,6 +254,18 @@
   </si>
   <si>
     <t xml:space="preserve">Ajouter un attribut for au label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">index.html + style.css</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage du texte non responsive sur petit écran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si le texte est trop long/l’écran pas assez large, il chevauche l’image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corriger le css (position relative)</t>
   </si>
 </sst>
 </file>
@@ -302,7 +323,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +334,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE7F5"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -350,7 +377,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -367,7 +394,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -405,7 +448,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCFE7F5"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -452,22 +495,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB92"/>
+  <dimension ref="A1:AB97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="80.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="80.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="9.61"/>
   </cols>
   <sheetData>
@@ -518,26 +561,29 @@
       <c r="AB1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="6" t="n">
         <v>1</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,7 +591,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2</v>
@@ -559,11 +605,14 @@
       <c r="F3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>9</v>
@@ -572,82 +621,96 @@
         <v>5</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="n">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>9</v>
@@ -656,151 +719,160 @@
         <v>8</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="n">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="0" t="s">
+      <c r="D10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="E10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="8" t="n">
         <v>1</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>21</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1" t="n">
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="5" t="n">
+      <c r="D14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="8" t="n">
         <v>1</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>9</v>
@@ -809,19 +881,19 @@
         <v>65</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>9</v>
@@ -830,19 +902,19 @@
         <v>74</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>9</v>
@@ -851,19 +923,19 @@
         <v>83</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>9</v>
@@ -872,19 +944,19 @@
         <v>136</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>9</v>
@@ -893,19 +965,19 @@
         <v>153</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>9</v>
@@ -914,19 +986,19 @@
         <v>205</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>9</v>
@@ -935,162 +1007,162 @@
         <v>220</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>34</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>61</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>83</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="G27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="1" t="n">
+      <c r="A28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="5" t="n">
+      <c r="D28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1105,15 +1177,15 @@
         <v>42</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -1126,36 +1198,36 @@
         <v>248</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G30" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="1" t="n">
+      <c r="A31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="4" t="n">
+      <c r="D31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" s="6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1170,15 +1242,15 @@
         <v>69</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G32" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
@@ -1191,15 +1263,15 @@
         <v>87</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -1212,15 +1284,15 @@
         <v>127</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G34" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -1233,15 +1305,15 @@
         <v>157</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G35" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -1254,15 +1326,15 @@
         <v>162</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G36" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -1275,15 +1347,15 @@
         <v>171</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G37" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="G37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
@@ -1296,15 +1368,15 @@
         <v>182</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G38" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
@@ -1317,40 +1389,40 @@
         <v>191</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G39" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>38</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G40" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="G40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>9</v>
@@ -1359,19 +1431,19 @@
         <v>52</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="G41" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="G41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>9</v>
@@ -1380,19 +1452,19 @@
         <v>55</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G42" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>9</v>
@@ -1401,19 +1473,19 @@
         <v>74</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G43" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>9</v>
@@ -1422,19 +1494,19 @@
         <v>144</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G44" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="G44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>9</v>
@@ -1443,40 +1515,40 @@
         <v>212</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G45" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>51</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G46" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>9</v>
@@ -1485,61 +1557,61 @@
         <v>44</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="1" t="n">
+      <c r="A49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="5" t="n">
         <v>254</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G49" s="0" t="n">
+      <c r="D49" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G49" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>9</v>
@@ -1548,18 +1620,18 @@
         <v>255</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>9</v>
@@ -1568,18 +1640,18 @@
         <v>256</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>9</v>
@@ -1588,18 +1660,18 @@
         <v>257</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>9</v>
@@ -1608,18 +1680,18 @@
         <v>263</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>9</v>
@@ -1628,18 +1700,18 @@
         <v>264</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>9</v>
@@ -1648,18 +1720,18 @@
         <v>265</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>9</v>
@@ -1668,18 +1740,18 @@
         <v>266</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>9</v>
@@ -1688,18 +1760,18 @@
         <v>267</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>9</v>
@@ -1708,18 +1780,18 @@
         <v>268</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>9</v>
@@ -1728,18 +1800,18 @@
         <v>269</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>9</v>
@@ -1748,18 +1820,18 @@
         <v>270</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>9</v>
@@ -1768,18 +1840,18 @@
         <v>271</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>9</v>
@@ -1788,18 +1860,18 @@
         <v>277</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>9</v>
@@ -1808,18 +1880,18 @@
         <v>278</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>9</v>
@@ -1828,18 +1900,18 @@
         <v>279</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>9</v>
@@ -1848,18 +1920,18 @@
         <v>280</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>9</v>
@@ -1868,18 +1940,18 @@
         <v>281</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>9</v>
@@ -1888,18 +1960,18 @@
         <v>282</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>9</v>
@@ -1908,18 +1980,18 @@
         <v>283</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>9</v>
@@ -1928,18 +2000,18 @@
         <v>284</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>9</v>
@@ -1948,176 +2020,179 @@
         <v>285</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C71" s="1" t="n">
+      <c r="A71" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="D71" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="F71" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="G71" s="0" t="n">
+      <c r="D71" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G71" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>12</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>13</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>16</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>17</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>18</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" s="1" t="n">
+      <c r="A77" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" s="5" t="n">
         <v>87</v>
       </c>
-      <c r="D77" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="F77" s="0" t="s">
-        <v>63</v>
+      <c r="D77" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G77" s="4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2128,7 +2203,7 @@
         <v>9</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>230</v>
+        <v>157</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>64</v>
@@ -2148,16 +2223,16 @@
         <v>9</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,16 +2243,16 @@
         <v>9</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,16 +2263,16 @@
         <v>9</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2205,19 +2280,19 @@
         <v>8</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>138</v>
+        <v>245</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,19 +2300,19 @@
         <v>8</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2245,19 +2320,19 @@
         <v>8</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2265,105 +2340,105 @@
         <v>8</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="D87" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D87" s="0" t="s">
+      <c r="E87" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="E87" s="0" t="s">
+      <c r="F87" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F87" s="0" t="s">
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G87" s="0" t="n">
+      <c r="D88" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G88" s="4" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D88" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E88" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F88" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C89" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="5" t="n">
         <v>85</v>
       </c>
-      <c r="D89" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E89" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F89" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="G89" s="0" t="n">
+      <c r="D90" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G90" s="4" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B90" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C90" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="D90" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E90" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F90" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,19 +2446,19 @@
         <v>8</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2391,19 +2466,119 @@
         <v>8</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C92" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="D92" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F92" s="0" t="s">
-        <v>74</v>
+      <c r="D93" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C94" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C95" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E95" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C96" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>